<commit_message>
fix change encoding and tempalate
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/2020/MARS KPIs.xlsx
+++ b/Projects/MARSRU_PROD/Data/2020/MARS KPIs.xlsx
@@ -20,15 +20,17 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$1</definedName>
-    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AC$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AC$65</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -456,7 +458,7 @@
     <t xml:space="preserve">BRAND in CAT</t>
   </si>
   <si>
-    <t xml:space="preserve">365 days, ARO, Every Day, Kotoffski, To Chto Nado, Lenta, BBCat, Dingo, Katty, TomCat, Tafi, Chammy, OKEY, Katty, Lapka, Nasha Marka, CTM, Pay less live better, Red Price, Круглый год</t>
+    <t xml:space="preserve">365 days, ARO, Every Day, Kotoffski, To Chto Nado, Lenta, BBCat, Dingo, Katty, TomCat, Tafi, Chammy, OKEY, Katty, Lapka, Nasha Marka, CTM, Pay less live better, Red Price</t>
   </si>
   <si>
     <t xml:space="preserve">Сум размер МАРС катег. собаки (в метрах) на всех полках (вкл лаком на осн полке)</t>
@@ -510,7 +512,7 @@
     <t xml:space="preserve">Availability of private brand in Dogs category</t>
   </si>
   <si>
-    <t xml:space="preserve">BBCat, Dingo, Katty,  Kotoffski, Pay less live better, TomCat, 365 days, ARO, CTM, Every Day, Lenta, Nasha Marka, Spar, To Chto Nado, Tafi, Chammy, OKEY, Red Price, Круглый год</t>
+    <t xml:space="preserve">BBCat, Dingo, Katty,  Kotoffski, Pay less live better, TomCat, 365 days, ARO, CTM, Every Day, Lenta, Nasha Marka, Spar, To Chto Nado, Tafi, Chammy, OKEY, Red Price</t>
   </si>
   <si>
     <t xml:space="preserve">Бренд-блок Whiskas - самый большой в категории</t>
@@ -1870,9 +1872,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="73.6963562753036"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3117408906883"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="74.3400809716599"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.246963562753"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2093,41 +2095,41 @@
   </sheetPr>
   <dimension ref="1:65"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G16" activeCellId="0" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.9352226720648"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.1012145748988"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.5910931174089"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.3076923076923"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6801619433198"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="61.587044534413"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="136.085020242915"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="36.6761133603239"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.165991902834"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.5344129554656"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.1943319838057"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="174.016194331984"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="27.8785425101215"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.9352226720648"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="52.2186234817814"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="29.9352226720648"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="26.165991902834"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="35.7651821862348"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="36.4493927125506"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="55.5303643724696"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="56.2145748987854"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="38.5060728744939"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="39.3036437246964"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="34.1619433198381"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="51.417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="62.1295546558704"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="137.327935222672"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="36.9554655870445"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="175.566801619433"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="52.7044534412956"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="36.0971659919028"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="36.7408906882591"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="56.663967611336"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="51.8461538461539"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.246963562753"/>
   </cols>
   <sheetData>
     <row r="1" s="10" customFormat="true" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6157,7 +6159,7 @@
       <c r="AC65" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC1"/>
+  <autoFilter ref="A1:AC65"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6182,35 +6184,35 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.3643724696356"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.5668016194332"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.5910931174089"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.3076923076923"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.336032388664"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6801619433198"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.5627530364373"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="130.255060728745"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.336032388664"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.165991902834"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.5344129554656"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.1943319838057"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.165991902834"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="27.8785425101215"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.9352226720648"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="52.2186234817814"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="24.1093117408907"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="22.0526315789474"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="35.7651821862348"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="36.4493927125506"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="55.5303643724696"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="56.2145748987854"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="38.5060728744939"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="39.3036437246964"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="34.1619433198381"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="51.417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.5627530364373"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="131.433198380567"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="30.1012145748988"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="52.7044534412956"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="24.3157894736842"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="36.0971659919028"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="36.7408906882591"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="56.0242914979757"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="56.663967611336"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="0" width="38.8825910931174"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="39.6356275303644"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="34.3846153846154"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="0" width="51.8461538461539"/>
+    <col collapsed="false" hidden="false" max="1025" min="30" style="0" width="11.246963562753"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7369,15 +7371,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8542510121458"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.9028340080972"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2550607287449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="56.9028340080972"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="15.7692307692308"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.1336032388664"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.71255060728745"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="57.417004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="9.74898785425101"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="39.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -26412,11 +26414,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.2550607287449"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.336032388664"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.7651821862348"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="56.9028340080972"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="22.7368421052632"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="57.417004048583"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28228,9 +28229,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.0769230769231"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.5627530364372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.246963562753"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28297,9 +28298,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.1983805668016"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.0526315789474"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="22.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.246963562753"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="33.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28350,10 +28351,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3117408906883"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="78.7246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.4817813765182"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.246963562753"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -28544,11 +28545,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.3076923076923"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7651821862348"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="35.9919028340081"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.246963562753"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>